<commit_message>
second floor boss and trap
</commit_message>
<xml_diff>
--- a/程序相关文档/第二层.xlsx
+++ b/程序相关文档/第二层.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18468" windowHeight="9924"/>
+    <workbookView windowWidth="18564" windowHeight="9347"/>
   </bookViews>
   <sheets>
     <sheet name="初始房间" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,6 +37,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -53,7 +84,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -74,10 +135,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -88,94 +158,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,43 +189,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,133 +327,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,50 +374,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -467,6 +416,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -481,150 +454,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -728,6 +721,45 @@
         <a:xfrm>
           <a:off x="77470" y="635"/>
           <a:ext cx="4582795" cy="6127115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2" descr="海天机关"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:srcRect t="34924" r="2566" b="10833"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4792980" y="723265"/>
+          <a:ext cx="6286500" cy="4679315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1028,8 +1060,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>